<commit_message>
Update figures and results
</commit_message>
<xml_diff>
--- a/2_real_read_tests/table_s2_real_read_results.xlsx
+++ b/2_real_read_tests/table_s2_real_read_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Trycycler/Paper_GitHub_repo/real_read_tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Trycycler/Paper_GitHub_repo/2_real_read_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42819F3-A85B-164E-AE4B-4ECBAAF2ABCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FFC8FD-BBDE-3449-B9B7-0B3AF8EDC50E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-840" yWindow="-24700" windowWidth="33600" windowHeight="19000" xr2:uid="{735A4778-CFAE-5E49-9105-BF0324A3A577}"/>
+    <workbookView xWindow="-3280" yWindow="-23520" windowWidth="36200" windowHeight="19000" xr2:uid="{735A4778-CFAE-5E49-9105-BF0324A3A577}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet descriptions" sheetId="14" r:id="rId1"/>
@@ -2048,7 +2048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="446">
+  <cellXfs count="445">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2741,9 +2741,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4207,9 +4204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAACD737-2C75-9143-B6E3-D8E9FD3FF1C3}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4237,7 +4232,7 @@
         <v>43</v>
       </c>
       <c r="H1" s="187" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -4565,7 +4560,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AL4" sqref="AL4"/>
+      <selection pane="bottomRight" activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4615,66 +4610,66 @@
   <sheetData>
     <row r="1" spans="1:41" ht="58" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="85"/>
-      <c r="B1" s="432" t="s">
+      <c r="B1" s="431" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="444"/>
-      <c r="D1" s="444"/>
-      <c r="E1" s="433"/>
-      <c r="F1" s="434" t="s">
+      <c r="C1" s="443"/>
+      <c r="D1" s="443"/>
+      <c r="E1" s="432"/>
+      <c r="F1" s="433" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="445"/>
-      <c r="H1" s="445"/>
-      <c r="I1" s="435"/>
-      <c r="J1" s="434" t="s">
+      <c r="G1" s="444"/>
+      <c r="H1" s="444"/>
+      <c r="I1" s="434"/>
+      <c r="J1" s="433" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="445"/>
-      <c r="L1" s="445"/>
-      <c r="M1" s="435"/>
-      <c r="N1" s="434" t="s">
+      <c r="K1" s="444"/>
+      <c r="L1" s="444"/>
+      <c r="M1" s="434"/>
+      <c r="N1" s="433" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="445"/>
-      <c r="P1" s="445"/>
-      <c r="Q1" s="435"/>
-      <c r="R1" s="437" t="s">
+      <c r="O1" s="444"/>
+      <c r="P1" s="444"/>
+      <c r="Q1" s="434"/>
+      <c r="R1" s="436" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="443"/>
-      <c r="T1" s="443"/>
-      <c r="U1" s="438"/>
-      <c r="V1" s="437" t="s">
+      <c r="S1" s="442"/>
+      <c r="T1" s="442"/>
+      <c r="U1" s="437"/>
+      <c r="V1" s="436" t="s">
         <v>88</v>
       </c>
-      <c r="W1" s="443"/>
-      <c r="X1" s="443"/>
-      <c r="Y1" s="438"/>
-      <c r="Z1" s="437" t="s">
+      <c r="W1" s="442"/>
+      <c r="X1" s="442"/>
+      <c r="Y1" s="437"/>
+      <c r="Z1" s="436" t="s">
         <v>89</v>
       </c>
-      <c r="AA1" s="443"/>
-      <c r="AB1" s="443"/>
-      <c r="AC1" s="438"/>
-      <c r="AD1" s="436" t="s">
+      <c r="AA1" s="442"/>
+      <c r="AB1" s="442"/>
+      <c r="AC1" s="437"/>
+      <c r="AD1" s="435" t="s">
         <v>90</v>
       </c>
-      <c r="AE1" s="430"/>
-      <c r="AF1" s="430"/>
-      <c r="AG1" s="431"/>
-      <c r="AH1" s="436" t="s">
+      <c r="AE1" s="429"/>
+      <c r="AF1" s="429"/>
+      <c r="AG1" s="430"/>
+      <c r="AH1" s="435" t="s">
         <v>91</v>
       </c>
-      <c r="AI1" s="430"/>
-      <c r="AJ1" s="430"/>
-      <c r="AK1" s="431"/>
-      <c r="AL1" s="430" t="s">
+      <c r="AI1" s="429"/>
+      <c r="AJ1" s="429"/>
+      <c r="AK1" s="430"/>
+      <c r="AL1" s="429" t="s">
         <v>92</v>
       </c>
-      <c r="AM1" s="430"/>
-      <c r="AN1" s="430"/>
-      <c r="AO1" s="431"/>
+      <c r="AM1" s="429"/>
+      <c r="AN1" s="429"/>
+      <c r="AO1" s="430"/>
     </row>
     <row r="2" spans="1:41" ht="61" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
@@ -5853,6 +5848,9 @@
     <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C9 E9 G9 I9 K9 M9 O9 Q9 S9 U9 W9 Y9 AA9:AO9" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -5872,13 +5870,13 @@
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="358"/>
       <c r="B1" s="371"/>
-      <c r="C1" s="386" t="s">
+      <c r="C1" s="385" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="387" t="s">
+      <c r="D1" s="386" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="387"/>
+      <c r="E1" s="386"/>
     </row>
     <row r="2" spans="1:5" ht="79" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="359" t="s">
@@ -5887,7 +5885,7 @@
       <c r="B2" s="372" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="386"/>
+      <c r="C2" s="385"/>
       <c r="D2" s="370" t="s">
         <v>7</v>
       </c>
@@ -6063,114 +6061,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="19" x14ac:dyDescent="0.25">
-      <c r="B1" s="388" t="s">
+      <c r="B1" s="387" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="388"/>
-      <c r="D1" s="388"/>
-      <c r="E1" s="388"/>
-      <c r="F1" s="388"/>
-      <c r="G1" s="388"/>
-      <c r="H1" s="388"/>
-      <c r="I1" s="388"/>
-      <c r="J1" s="388"/>
-      <c r="K1" s="388"/>
-      <c r="L1" s="388"/>
-      <c r="M1" s="389"/>
-      <c r="N1" s="390" t="s">
+      <c r="C1" s="387"/>
+      <c r="D1" s="387"/>
+      <c r="E1" s="387"/>
+      <c r="F1" s="387"/>
+      <c r="G1" s="387"/>
+      <c r="H1" s="387"/>
+      <c r="I1" s="387"/>
+      <c r="J1" s="387"/>
+      <c r="K1" s="387"/>
+      <c r="L1" s="387"/>
+      <c r="M1" s="388"/>
+      <c r="N1" s="389" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="391"/>
-      <c r="P1" s="391"/>
-      <c r="Q1" s="391"/>
-      <c r="R1" s="391"/>
-      <c r="S1" s="391"/>
-      <c r="T1" s="391"/>
-      <c r="U1" s="391"/>
-      <c r="V1" s="391"/>
-      <c r="W1" s="391"/>
-      <c r="X1" s="391"/>
-      <c r="Y1" s="392"/>
+      <c r="O1" s="390"/>
+      <c r="P1" s="390"/>
+      <c r="Q1" s="390"/>
+      <c r="R1" s="390"/>
+      <c r="S1" s="390"/>
+      <c r="T1" s="390"/>
+      <c r="U1" s="390"/>
+      <c r="V1" s="390"/>
+      <c r="W1" s="390"/>
+      <c r="X1" s="390"/>
+      <c r="Y1" s="391"/>
     </row>
     <row r="2" spans="1:25" s="85" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="411" t="s">
+      <c r="B2" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="412"/>
-      <c r="D2" s="412"/>
-      <c r="E2" s="412"/>
-      <c r="F2" s="412"/>
-      <c r="G2" s="412"/>
-      <c r="H2" s="403" t="s">
+      <c r="C2" s="411"/>
+      <c r="D2" s="411"/>
+      <c r="E2" s="411"/>
+      <c r="F2" s="411"/>
+      <c r="G2" s="411"/>
+      <c r="H2" s="402" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="404"/>
-      <c r="J2" s="404"/>
-      <c r="K2" s="404"/>
-      <c r="L2" s="404"/>
-      <c r="M2" s="405"/>
-      <c r="N2" s="390" t="s">
+      <c r="I2" s="403"/>
+      <c r="J2" s="403"/>
+      <c r="K2" s="403"/>
+      <c r="L2" s="403"/>
+      <c r="M2" s="404"/>
+      <c r="N2" s="389" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="391"/>
-      <c r="P2" s="391"/>
-      <c r="Q2" s="391"/>
-      <c r="R2" s="391"/>
-      <c r="S2" s="391"/>
-      <c r="T2" s="393" t="s">
+      <c r="O2" s="390"/>
+      <c r="P2" s="390"/>
+      <c r="Q2" s="390"/>
+      <c r="R2" s="390"/>
+      <c r="S2" s="390"/>
+      <c r="T2" s="392" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="394"/>
-      <c r="V2" s="394"/>
-      <c r="W2" s="394"/>
-      <c r="X2" s="394"/>
-      <c r="Y2" s="395"/>
+      <c r="U2" s="393"/>
+      <c r="V2" s="393"/>
+      <c r="W2" s="393"/>
+      <c r="X2" s="393"/>
+      <c r="Y2" s="394"/>
     </row>
     <row r="3" spans="1:25" s="85" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="409" t="s">
+      <c r="B3" s="408" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="410"/>
-      <c r="D3" s="410"/>
-      <c r="E3" s="401" t="s">
+      <c r="C3" s="409"/>
+      <c r="D3" s="409"/>
+      <c r="E3" s="400" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="410"/>
-      <c r="G3" s="410"/>
-      <c r="H3" s="406" t="s">
+      <c r="F3" s="409"/>
+      <c r="G3" s="409"/>
+      <c r="H3" s="405" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="407"/>
-      <c r="J3" s="408" t="s">
+      <c r="I3" s="406"/>
+      <c r="J3" s="407" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="407"/>
-      <c r="L3" s="401" t="s">
+      <c r="K3" s="406"/>
+      <c r="L3" s="400" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="402"/>
-      <c r="N3" s="413" t="s">
+      <c r="M3" s="401"/>
+      <c r="N3" s="412" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="414"/>
-      <c r="P3" s="414"/>
-      <c r="Q3" s="399" t="s">
+      <c r="O3" s="413"/>
+      <c r="P3" s="413"/>
+      <c r="Q3" s="398" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="414"/>
-      <c r="S3" s="414"/>
-      <c r="T3" s="396" t="s">
+      <c r="R3" s="413"/>
+      <c r="S3" s="413"/>
+      <c r="T3" s="395" t="s">
         <v>1</v>
       </c>
-      <c r="U3" s="397"/>
-      <c r="V3" s="398" t="s">
+      <c r="U3" s="396"/>
+      <c r="V3" s="397" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="397"/>
-      <c r="X3" s="399" t="s">
+      <c r="W3" s="396"/>
+      <c r="X3" s="398" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="400"/>
+      <c r="Y3" s="399"/>
     </row>
     <row r="4" spans="1:25" s="86" customFormat="1" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
@@ -6823,10 +6821,10 @@
   <dimension ref="A1:AY9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6885,76 +6883,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" s="104" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="421" t="s">
+      <c r="B1" s="420" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="422"/>
-      <c r="D1" s="422"/>
-      <c r="E1" s="422"/>
-      <c r="F1" s="423"/>
-      <c r="G1" s="421" t="s">
+      <c r="C1" s="421"/>
+      <c r="D1" s="421"/>
+      <c r="E1" s="421"/>
+      <c r="F1" s="422"/>
+      <c r="G1" s="420" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="422"/>
-      <c r="I1" s="422"/>
-      <c r="J1" s="422"/>
-      <c r="K1" s="423"/>
-      <c r="L1" s="427" t="s">
+      <c r="H1" s="421"/>
+      <c r="I1" s="421"/>
+      <c r="J1" s="421"/>
+      <c r="K1" s="422"/>
+      <c r="L1" s="426" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="428"/>
-      <c r="N1" s="428"/>
-      <c r="O1" s="428"/>
-      <c r="P1" s="429"/>
-      <c r="Q1" s="427" t="s">
+      <c r="M1" s="427"/>
+      <c r="N1" s="427"/>
+      <c r="O1" s="427"/>
+      <c r="P1" s="428"/>
+      <c r="Q1" s="426" t="s">
         <v>70</v>
       </c>
-      <c r="R1" s="428"/>
-      <c r="S1" s="428"/>
-      <c r="T1" s="428"/>
-      <c r="U1" s="429"/>
-      <c r="V1" s="424" t="s">
+      <c r="R1" s="427"/>
+      <c r="S1" s="427"/>
+      <c r="T1" s="427"/>
+      <c r="U1" s="428"/>
+      <c r="V1" s="423" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="425"/>
-      <c r="X1" s="425"/>
-      <c r="Y1" s="425"/>
-      <c r="Z1" s="426"/>
-      <c r="AA1" s="424" t="s">
+      <c r="W1" s="424"/>
+      <c r="X1" s="424"/>
+      <c r="Y1" s="424"/>
+      <c r="Z1" s="425"/>
+      <c r="AA1" s="423" t="s">
         <v>72</v>
       </c>
-      <c r="AB1" s="425"/>
-      <c r="AC1" s="425"/>
-      <c r="AD1" s="425"/>
-      <c r="AE1" s="426"/>
-      <c r="AF1" s="415" t="s">
+      <c r="AB1" s="424"/>
+      <c r="AC1" s="424"/>
+      <c r="AD1" s="424"/>
+      <c r="AE1" s="425"/>
+      <c r="AF1" s="414" t="s">
         <v>73</v>
       </c>
-      <c r="AG1" s="416"/>
-      <c r="AH1" s="416"/>
-      <c r="AI1" s="416"/>
-      <c r="AJ1" s="417"/>
-      <c r="AK1" s="415" t="s">
+      <c r="AG1" s="415"/>
+      <c r="AH1" s="415"/>
+      <c r="AI1" s="415"/>
+      <c r="AJ1" s="416"/>
+      <c r="AK1" s="414" t="s">
         <v>74</v>
       </c>
-      <c r="AL1" s="416"/>
-      <c r="AM1" s="416"/>
-      <c r="AN1" s="416"/>
-      <c r="AO1" s="417"/>
-      <c r="AP1" s="418" t="s">
+      <c r="AL1" s="415"/>
+      <c r="AM1" s="415"/>
+      <c r="AN1" s="415"/>
+      <c r="AO1" s="416"/>
+      <c r="AP1" s="417" t="s">
         <v>75</v>
       </c>
-      <c r="AQ1" s="419"/>
-      <c r="AR1" s="419"/>
-      <c r="AS1" s="419"/>
-      <c r="AT1" s="420"/>
-      <c r="AU1" s="418" t="s">
+      <c r="AQ1" s="418"/>
+      <c r="AR1" s="418"/>
+      <c r="AS1" s="418"/>
+      <c r="AT1" s="419"/>
+      <c r="AU1" s="417" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" s="419"/>
-      <c r="AW1" s="419"/>
-      <c r="AX1" s="419"/>
-      <c r="AY1" s="420"/>
+      <c r="AV1" s="418"/>
+      <c r="AW1" s="418"/>
+      <c r="AX1" s="418"/>
+      <c r="AY1" s="419"/>
     </row>
     <row r="2" spans="1:51" s="86" customFormat="1" ht="74" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
@@ -8220,17 +8218,17 @@
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="378" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="377" t="s">
+    <row r="1" spans="1:4" s="377" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="379" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="380" t="s">
+      <c r="B1" s="379" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="380" t="s">
+      <c r="C1" s="379" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="380" t="s">
+      <c r="D1" s="379" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8238,11 +8236,11 @@
       <c r="A2" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="381">
+      <c r="B2" s="380">
         <v>-1</v>
       </c>
-      <c r="C2" s="381"/>
-      <c r="D2" s="381" t="s">
+      <c r="C2" s="380"/>
+      <c r="D2" s="380" t="s">
         <v>127</v>
       </c>
     </row>
@@ -8250,11 +8248,11 @@
       <c r="A3" s="166" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="382">
+      <c r="B3" s="381">
         <v>-2</v>
       </c>
-      <c r="C3" s="382"/>
-      <c r="D3" s="382" t="s">
+      <c r="C3" s="381"/>
+      <c r="D3" s="381" t="s">
         <v>112</v>
       </c>
     </row>
@@ -8262,21 +8260,21 @@
       <c r="A4" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="383">
+      <c r="B4" s="382">
         <v>0</v>
       </c>
-      <c r="C4" s="383"/>
-      <c r="D4" s="383"/>
+      <c r="C4" s="382"/>
+      <c r="D4" s="382"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="383">
+      <c r="B5" s="382">
         <v>-4</v>
       </c>
-      <c r="C5" s="383"/>
-      <c r="D5" s="383" t="s">
+      <c r="C5" s="382"/>
+      <c r="D5" s="382" t="s">
         <v>128</v>
       </c>
     </row>
@@ -8284,23 +8282,23 @@
       <c r="A6" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="383">
+      <c r="B6" s="382">
         <v>1</v>
       </c>
-      <c r="C6" s="383" t="s">
+      <c r="C6" s="382" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="383"/>
+      <c r="D6" s="382"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="383">
+      <c r="B7" s="382">
         <v>-4</v>
       </c>
-      <c r="C7" s="383"/>
-      <c r="D7" s="383" t="s">
+      <c r="C7" s="382"/>
+      <c r="D7" s="382" t="s">
         <v>129</v>
       </c>
     </row>
@@ -8308,33 +8306,33 @@
       <c r="A8" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="383">
+      <c r="B8" s="382">
         <v>0</v>
       </c>
-      <c r="C8" s="383"/>
-      <c r="D8" s="383"/>
+      <c r="C8" s="382"/>
+      <c r="D8" s="382"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="383">
+      <c r="B9" s="382">
         <v>4</v>
       </c>
-      <c r="C9" s="383" t="s">
+      <c r="C9" s="382" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="383"/>
+      <c r="D9" s="382"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="383">
+      <c r="B10" s="382">
         <v>-9</v>
       </c>
-      <c r="C10" s="383"/>
-      <c r="D10" s="383" t="s">
+      <c r="C10" s="382"/>
+      <c r="D10" s="382" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8342,11 +8340,11 @@
       <c r="A11" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="383">
+      <c r="B11" s="382">
         <v>-1</v>
       </c>
-      <c r="C11" s="383"/>
-      <c r="D11" s="383" t="s">
+      <c r="C11" s="382"/>
+      <c r="D11" s="382" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8354,11 +8352,11 @@
       <c r="A12" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="384">
+      <c r="B12" s="383">
         <v>-4</v>
       </c>
-      <c r="C12" s="384"/>
-      <c r="D12" s="384" t="s">
+      <c r="C12" s="383"/>
+      <c r="D12" s="383" t="s">
         <v>132</v>
       </c>
     </row>
@@ -8366,11 +8364,11 @@
       <c r="A13" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="385">
+      <c r="B13" s="384">
         <v>-13</v>
       </c>
-      <c r="C13" s="385"/>
-      <c r="D13" s="385" t="s">
+      <c r="C13" s="384"/>
+      <c r="D13" s="384" t="s">
         <v>133</v>
       </c>
     </row>
@@ -8380,7 +8378,7 @@
       <c r="D14" s="366"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="379" t="s">
+      <c r="A15" s="378" t="s">
         <v>113</v>
       </c>
       <c r="B15" s="366" cm="1">
@@ -8404,7 +8402,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AF3" sqref="AF3:AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8445,70 +8443,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="85" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="432" t="s">
+      <c r="B1" s="431" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="433"/>
-      <c r="D1" s="441" t="s">
+      <c r="C1" s="432"/>
+      <c r="D1" s="440" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="442"/>
-      <c r="F1" s="441" t="s">
+      <c r="E1" s="441"/>
+      <c r="F1" s="440" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="442"/>
-      <c r="H1" s="441" t="s">
+      <c r="G1" s="441"/>
+      <c r="H1" s="440" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="442"/>
-      <c r="J1" s="439" t="s">
+      <c r="I1" s="441"/>
+      <c r="J1" s="438" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="440"/>
-      <c r="L1" s="439" t="s">
+      <c r="K1" s="439"/>
+      <c r="L1" s="438" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="440"/>
-      <c r="N1" s="439" t="s">
+      <c r="M1" s="439"/>
+      <c r="N1" s="438" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="440"/>
-      <c r="P1" s="434" t="s">
+      <c r="O1" s="439"/>
+      <c r="P1" s="433" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="435"/>
-      <c r="R1" s="434" t="s">
+      <c r="Q1" s="434"/>
+      <c r="R1" s="433" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="435"/>
-      <c r="T1" s="434" t="s">
+      <c r="S1" s="434"/>
+      <c r="T1" s="433" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="435"/>
-      <c r="V1" s="437" t="s">
+      <c r="U1" s="434"/>
+      <c r="V1" s="436" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="438"/>
-      <c r="X1" s="437" t="s">
+      <c r="W1" s="437"/>
+      <c r="X1" s="436" t="s">
         <v>88</v>
       </c>
-      <c r="Y1" s="438"/>
-      <c r="Z1" s="437" t="s">
+      <c r="Y1" s="437"/>
+      <c r="Z1" s="436" t="s">
         <v>89</v>
       </c>
-      <c r="AA1" s="438"/>
-      <c r="AB1" s="436" t="s">
+      <c r="AA1" s="437"/>
+      <c r="AB1" s="435" t="s">
         <v>90</v>
       </c>
-      <c r="AC1" s="431"/>
-      <c r="AD1" s="436" t="s">
+      <c r="AC1" s="430"/>
+      <c r="AD1" s="435" t="s">
         <v>91</v>
       </c>
-      <c r="AE1" s="431"/>
-      <c r="AF1" s="430" t="s">
+      <c r="AE1" s="430"/>
+      <c r="AF1" s="429" t="s">
         <v>92</v>
       </c>
-      <c r="AG1" s="431"/>
+      <c r="AG1" s="430"/>
       <c r="AH1" s="20"/>
     </row>
     <row r="2" spans="1:34" s="86" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.3">
@@ -9216,7 +9214,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E52B5EA-0D5A-5747-9340-A15820583CFB}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>